<commit_message>
Graph theory measurements and visualizations
</commit_message>
<xml_diff>
--- a/Extra/QueryComparisons.xlsx
+++ b/Extra/QueryComparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jyrki\Documents\GitHub\LDAC2022_Dataset\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB31F9B-87E6-44BF-A0C2-29253351A2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC03DBD4-8FE4-45C5-B546-B2D0DFFB8752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{814C8306-D283-4CA1-964E-4283804CA8D7}"/>
+    <workbookView xWindow="-1778" yWindow="1418" windowWidth="21585" windowHeight="13664" xr2:uid="{814C8306-D283-4CA1-964E-4283804CA8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
   <si>
     <t>Events</t>
   </si>
@@ -427,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -479,6 +479,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E301BC51-C7D2-4337-AAD2-5DE1E86EF203}">
   <dimension ref="B5:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F22"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1010,7 +1015,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>38</v>
@@ -1027,16 +1032,16 @@
         <v>54</v>
       </c>
       <c r="C14" s="19">
-        <v>2.77</v>
+        <v>2.69</v>
       </c>
       <c r="D14" s="19">
-        <v>3.18</v>
+        <v>2.7</v>
       </c>
       <c r="E14" s="19">
-        <v>3.11</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="F14" s="20">
-        <v>3.43</v>
+        <v>2.79</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>10</v>
@@ -1053,16 +1058,16 @@
         <v>60</v>
       </c>
       <c r="C15" s="2">
-        <v>1.75</v>
+        <v>1.78</v>
       </c>
       <c r="D15" s="2">
-        <v>2.96</v>
+        <v>2.88</v>
       </c>
       <c r="E15" s="2">
-        <v>3.03</v>
+        <v>2.76</v>
       </c>
       <c r="F15" s="9">
-        <v>2.65</v>
+        <v>2.6</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>6</v>
@@ -1082,13 +1087,13 @@
         <v>0.09</v>
       </c>
       <c r="D16" s="28">
-        <v>0.2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E16" s="28">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="F16" s="29">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>8</v>
@@ -1105,10 +1110,10 @@
         <v>58</v>
       </c>
       <c r="C17" s="27">
-        <v>0.13</v>
+        <v>0.06</v>
       </c>
       <c r="D17" s="19">
-        <v>0.44</v>
+        <v>0.2</v>
       </c>
       <c r="E17" s="19">
         <v>0</v>
@@ -1131,10 +1136,10 @@
         <v>59</v>
       </c>
       <c r="C18" s="4">
-        <v>0.06</v>
+        <v>2.7E-2</v>
       </c>
       <c r="D18" s="3">
-        <v>0.22</v>
+        <v>0.08</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
@@ -1338,7 +1343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="H33" s="5" t="s">
         <v>17</v>
       </c>
@@ -1349,7 +1354,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="H34" s="5" t="s">
         <v>18</v>
       </c>
@@ -1360,7 +1365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="H35" s="5" t="s">
         <v>19</v>
       </c>
@@ -1371,7 +1376,22 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="H36" s="5" t="s">
         <v>20</v>
       </c>
@@ -1382,7 +1402,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B37" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="19">
+        <v>29</v>
+      </c>
+      <c r="D37" s="19">
+        <v>14</v>
+      </c>
+      <c r="E37" s="19">
+        <v>21</v>
+      </c>
+      <c r="F37" s="20">
+        <v>24</v>
+      </c>
       <c r="H37" s="5" t="s">
         <v>22</v>
       </c>
@@ -1393,7 +1428,22 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="2">
+        <v>12</v>
+      </c>
+      <c r="D38" s="2">
+        <v>8</v>
+      </c>
+      <c r="E38" s="2">
+        <v>7</v>
+      </c>
+      <c r="F38" s="9">
+        <v>13</v>
+      </c>
       <c r="H38" s="5" t="s">
         <v>23</v>
       </c>
@@ -1402,7 +1452,22 @@
       </c>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="2">
+        <v>15</v>
+      </c>
+      <c r="D39" s="2">
+        <v>9</v>
+      </c>
+      <c r="E39" s="2">
+        <v>7</v>
+      </c>
+      <c r="F39" s="9">
+        <v>17</v>
+      </c>
       <c r="H39" s="5" t="s">
         <v>24</v>
       </c>
@@ -1411,7 +1476,22 @@
       </c>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="3">
+        <v>57</v>
+      </c>
+      <c r="D40" s="3">
+        <v>31</v>
+      </c>
+      <c r="E40" s="3">
+        <v>35</v>
+      </c>
+      <c r="F40" s="11">
+        <v>54</v>
+      </c>
       <c r="H40" s="3" t="s">
         <v>29</v>
       </c>
@@ -1420,52 +1500,169 @@
       </c>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="42" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="13">
+        <v>3</v>
+      </c>
+      <c r="D41" s="13">
+        <v>2</v>
+      </c>
+      <c r="E41" s="13">
+        <v>3</v>
+      </c>
+      <c r="F41" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B42" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="19">
+        <v>4</v>
+      </c>
+      <c r="D42" s="19">
+        <v>3</v>
+      </c>
+      <c r="E42" s="19">
+        <v>4</v>
+      </c>
+      <c r="F42" s="20">
+        <v>4</v>
+      </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B43" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="2">
+        <v>6</v>
+      </c>
+      <c r="D43" s="2">
+        <v>4</v>
+      </c>
+      <c r="E43" s="2">
+        <v>5</v>
+      </c>
+      <c r="F43" s="9">
+        <v>6</v>
+      </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B44" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="20"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="8" t="str">
+        <f>"- the current state"</f>
+        <v>- the current state</v>
+      </c>
+      <c r="C45" s="2">
+        <v>9</v>
+      </c>
+      <c r="D45" s="2">
+        <v>6</v>
+      </c>
+      <c r="E45" s="2">
+        <v>6</v>
+      </c>
+      <c r="F45" s="9">
+        <v>6</v>
+      </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B46" s="8" t="str">
+        <f>"- state at a specific time"</f>
+        <v>- state at a specific time</v>
+      </c>
+      <c r="C46" s="2">
+        <v>9</v>
+      </c>
+      <c r="D46" s="2">
+        <v>6</v>
+      </c>
+      <c r="E46" s="2">
+        <v>6</v>
+      </c>
+      <c r="F46" s="9">
+        <v>6</v>
+      </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B47" s="10" t="str">
+        <f>"- state at initial time"</f>
+        <v>- state at initial time</v>
+      </c>
+      <c r="C47" s="3">
+        <v>6</v>
+      </c>
+      <c r="D47" s="3">
+        <v>3</v>
+      </c>
+      <c r="E47" s="3">
+        <v>4</v>
+      </c>
+      <c r="F47" s="11">
+        <v>5</v>
+      </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="32"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
     </row>
-    <row r="50" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="51" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="52" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="53" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="54" spans="8:10" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="50" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="31"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+    </row>
+    <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="53" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Source code and updated table
</commit_message>
<xml_diff>
--- a/Extra/QueryComparisons.xlsx
+++ b/Extra/QueryComparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jyrki\Documents\GitHub\LDAC2022_Dataset\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC03DBD4-8FE4-45C5-B546-B2D0DFFB8752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB7E14E-96E4-465D-8F9F-241058B6114C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1778" yWindow="1418" windowWidth="21585" windowHeight="13664" xr2:uid="{814C8306-D283-4CA1-964E-4283804CA8D7}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{814C8306-D283-4CA1-964E-4283804CA8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
   <si>
     <t>Events</t>
   </si>
@@ -221,13 +221,28 @@
   </si>
   <si>
     <t>Max. steps to a leaf. UnweightedEccentricity for a topic.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triples at the end when modification steps combined </t>
+  </si>
+  <si>
+    <t>Final graph: reified model diameter</t>
+  </si>
+  <si>
+    <t>Final graph: connected components Model not reified</t>
+  </si>
+  <si>
+    <t>Max. steps to a leaf. Reified model UnweightedEccentricity for a topic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial graph: reified model diameter </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +262,22 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -427,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -480,10 +511,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E301BC51-C7D2-4337-AAD2-5DE1E86EF203}">
   <dimension ref="B5:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:F47"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1376,7 +1413,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B36" s="14" t="s">
         <v>1</v>
       </c>
@@ -1409,7 +1446,7 @@
       <c r="C37" s="19">
         <v>29</v>
       </c>
-      <c r="D37" s="19">
+      <c r="D37" s="37">
         <v>14</v>
       </c>
       <c r="E37" s="19">
@@ -1435,10 +1472,10 @@
       <c r="C38" s="2">
         <v>12</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="38">
         <v>8</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="38">
         <v>7</v>
       </c>
       <c r="F38" s="9">
@@ -1459,10 +1496,10 @@
       <c r="C39" s="2">
         <v>15</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="38">
         <v>9</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="38">
         <v>7</v>
       </c>
       <c r="F39" s="9">
@@ -1480,16 +1517,16 @@
       <c r="B40" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="34">
         <v>57</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="35">
         <v>31</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="35">
         <v>35</v>
       </c>
-      <c r="F40" s="11">
+      <c r="F40" s="40">
         <v>54</v>
       </c>
       <c r="H40" s="3" t="s">
@@ -1501,153 +1538,173 @@
       <c r="J40" s="3"/>
     </row>
     <row r="41" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B41" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="13">
+      <c r="B41" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="32">
+        <v>46</v>
+      </c>
+      <c r="D41" s="32">
+        <v>23</v>
+      </c>
+      <c r="E41" s="32">
+        <v>35</v>
+      </c>
+      <c r="F41" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B42" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="13">
         <v>3</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D42" s="36">
         <v>2</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E42" s="13">
         <v>3</v>
       </c>
-      <c r="F41" s="12">
+      <c r="F42" s="12">
         <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="19">
-        <v>4</v>
-      </c>
-      <c r="D42" s="19">
-        <v>3</v>
-      </c>
-      <c r="E42" s="19">
-        <v>4</v>
-      </c>
-      <c r="F42" s="20">
-        <v>4</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
     <row r="43" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="2">
-        <v>6</v>
-      </c>
-      <c r="D43" s="2">
+      <c r="B43" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="19">
         <v>4</v>
       </c>
-      <c r="E43" s="2">
-        <v>5</v>
-      </c>
-      <c r="F43" s="9">
-        <v>6</v>
+      <c r="D43" s="37">
+        <v>3</v>
+      </c>
+      <c r="E43" s="19">
+        <v>4</v>
+      </c>
+      <c r="F43" s="20">
+        <v>4</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B44" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="20"/>
+      <c r="B44" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="39">
+        <v>6</v>
+      </c>
+      <c r="D44" s="38">
+        <v>4</v>
+      </c>
+      <c r="E44" s="2">
+        <v>5</v>
+      </c>
+      <c r="F44" s="41">
+        <v>6</v>
+      </c>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="8" t="str">
-        <f>"- the current state"</f>
-        <v>- the current state</v>
-      </c>
-      <c r="C45" s="2">
-        <v>9</v>
-      </c>
-      <c r="D45" s="2">
-        <v>6</v>
-      </c>
-      <c r="E45" s="2">
-        <v>6</v>
-      </c>
-      <c r="F45" s="9">
-        <v>6</v>
+    <row r="45" spans="2:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B45" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="36">
+        <v>1</v>
+      </c>
+      <c r="D45" s="36">
+        <v>1</v>
+      </c>
+      <c r="E45" s="13">
+        <v>23</v>
+      </c>
+      <c r="F45" s="12">
+        <v>8</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
     <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="8" t="str">
-        <f>"- state at a specific time"</f>
-        <v>- state at a specific time</v>
-      </c>
-      <c r="C46" s="2">
-        <v>9</v>
-      </c>
-      <c r="D46" s="2">
-        <v>6</v>
-      </c>
-      <c r="E46" s="2">
-        <v>6</v>
-      </c>
-      <c r="F46" s="9">
-        <v>6</v>
-      </c>
+      <c r="B46" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="20"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B47" s="10" t="str">
-        <f>"- state at initial time"</f>
-        <v>- state at initial time</v>
-      </c>
-      <c r="C47" s="3">
-        <v>6</v>
-      </c>
-      <c r="D47" s="3">
-        <v>3</v>
-      </c>
-      <c r="E47" s="3">
-        <v>4</v>
-      </c>
-      <c r="F47" s="11">
-        <v>5</v>
+      <c r="B47" s="8" t="str">
+        <f>"- the current state"</f>
+        <v>- the current state</v>
+      </c>
+      <c r="C47" s="39">
+        <v>9</v>
+      </c>
+      <c r="D47" s="2">
+        <v>6</v>
+      </c>
+      <c r="E47" s="2">
+        <v>6</v>
+      </c>
+      <c r="F47" s="9">
+        <v>6</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
     <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
+      <c r="B48" s="8" t="str">
+        <f>"- state at a specific time"</f>
+        <v>- state at a specific time</v>
+      </c>
+      <c r="C48" s="39">
+        <v>9</v>
+      </c>
+      <c r="D48" s="2">
+        <v>6</v>
+      </c>
+      <c r="E48" s="2">
+        <v>6</v>
+      </c>
+      <c r="F48" s="9">
+        <v>6</v>
+      </c>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
     <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B49" s="32"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
+      <c r="B49" s="10" t="str">
+        <f>"- state at initial time"</f>
+        <v>- state at initial time</v>
+      </c>
+      <c r="C49" s="3">
+        <v>6</v>
+      </c>
+      <c r="D49" s="35">
+        <v>3</v>
+      </c>
+      <c r="E49" s="35">
+        <v>4</v>
+      </c>
+      <c r="F49" s="11">
+        <v>5</v>
+      </c>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>

</xml_diff>